<commit_message>
error handling and specific search results
</commit_message>
<xml_diff>
--- a/ExcelSelenium/src/test/resources/amazonData.xlsx
+++ b/ExcelSelenium/src/test/resources/amazonData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
   <si>
     <t>Cat</t>
   </si>
@@ -43,49 +43,73 @@
     <t>Fieajfiojeaiofj</t>
   </si>
   <si>
-    <t>SmartFeeder Automatic Pet Feeder</t>
-  </si>
-  <si>
-    <t>Flexible Colored Drinking Straws | Disposable Bendy Plastic Straws | Party Straws | Colorful Straws for Kids | Party Goods Pack | BPA Free |450 Count</t>
-  </si>
-  <si>
-    <t>AmazonBasics Copy Paper - 96 Bright, 8.5" x 11", 1 Ream (500 Sheets) (AZ851120HB1R)</t>
-  </si>
-  <si>
-    <t>2 Pack Bed Pillows for Sleeping-Hypoallergenic Pillow for Side and Back Sleeper Hotel Pillows Down Alternative Sleeping Pillows with Super Soft Plush Fiber Fill-Queen Size</t>
-  </si>
-  <si>
-    <t>Giantex 4'x10'x2 Gymnastics Mat Thick Folding Panel for Gym Fitness with Hook &amp; Loop Fasteners</t>
-  </si>
-  <si>
-    <t>Hiware 12-piece Dinner Forks Set, 8 Inches, Extra-Fine 18/8 Stainless Steel</t>
-  </si>
-  <si>
-    <t>DOWAN 29 Ounce Porcelain Soup Bowls - 3 Packs, Stackable Round, White</t>
-  </si>
-  <si>
-    <t>Clear Plastic Disposable Cups | 14 oz. 100 Pack | Tall Plastic Glasses | Party Tumbler Cups | Heavy Duty Hard Plastic Cups | For Wine, Champagne, Cocktails, Beer, Water [Drinket Collection]</t>
-  </si>
-  <si>
-    <t>Bedsure Flannel Fleece Luxury Blanket Grey Throw Lightweight Cozy Plush Microfiber Solid Blanket</t>
+    <t>AmazonBasics Cat Activity Tree with Scratching Posts, Medium</t>
+  </si>
+  <si>
+    <t>EZ Straw Just Straw Clean Processed Straw, Small Bale (1 cubic foot bale)</t>
+  </si>
+  <si>
+    <t>AmazonBasics 92 Bright Multipurpose Copy Paper - 8.5 x 11 Inches, 10 Ream Case (5,000 Sheets)</t>
+  </si>
+  <si>
+    <t>Perfect Cloud Double Airflow Memory Foam Pillow Featuring Cooling Ventilated Visco Foam Core and Mesh Trim for a Refreshing Sleeping Experience</t>
+  </si>
+  <si>
+    <t>AmazonBasics 1/2-Inch Extra Thick Exercise Mat</t>
+  </si>
+  <si>
+    <t>Dinner Forks,MCIRCO 12-Piece Good Quality Stainless Steel Table Forks Cutlery Set,8 Inch</t>
+  </si>
+  <si>
+    <t>DOWAN 1-1/2 Quart Porcelain Serving Bowls, 2-Pack</t>
+  </si>
+  <si>
+    <t>Amazon Brand - Solimo 18oz Disposable Plastic Party Cups, 200 Count, Red</t>
+  </si>
+  <si>
+    <t>BEDSURE Sherpa Fleece Blanket Twin Size Red Plush Throw Blanket Fuzzy Soft Blanket Microfiber</t>
   </si>
   <si>
     <t>No Item Found</t>
   </si>
   <si>
-    <t>YOGALAND Premium Yoga Mat with Carrier Strap - Yoga Mat 6mm 1/4-Inch Thick, Non-Slip, Eco-Friendly, Lightweight, Extra Large 72" x 24" for Yoga Pilates Fitness Exercise</t>
-  </si>
-  <si>
-    <t>Dinner Forks, MCIRCO 18/10 Heavy-duty Stainless Steel Dinner Forks Set of 8, 8 Inches</t>
-  </si>
-  <si>
-    <t>Ohm Store Tibetan Singing Bowl Set - Helpful for Meditation, Yoga, Relaxation, Chakra Healing &amp; Stress Relief</t>
-  </si>
-  <si>
-    <t>Balichun Luxury 330 GSM Fleece Blanket Super Soft Warm Fuzzy Lightweight Bed or Couch Blanket Twin/Queen/King Size(Queen,Dark Grey)</t>
-  </si>
-  <si>
-    <t>DOZZZ Oversize Flannel Polar Fleece Throw Blanket 70 x 50 Fuzzy Plush Microfiber for Couch Cover Sofa Chair Bed</t>
+    <t>Utopia Bedding Premium Fiber Filled Bed Pillows for Sleeping - Pack of 2 - Super Plush Pillows - Soft and Fluffy Queen Sized Pillows</t>
+  </si>
+  <si>
+    <t>AmazonBasics Stainless Steel Dinner Forks with Scalloped Edge, Pack of 12</t>
+  </si>
+  <si>
+    <t>Bedsure Flannel Fleece Luxury Blanket Navy Twin Size Lightweight Cozy Plush Microfiber Solid Blanket</t>
+  </si>
+  <si>
+    <t>Coop Home Goods - PREMIUM Adjustable Loft - Shredded Hypoallergenic Certipur Memory Foam Pillow with washable removable cover - 20 x 30 - Queen size</t>
+  </si>
+  <si>
+    <t>Bare Home Ultra Soft Microplush Velvet Blanket - Luxurious Fuzzy Fleece Fur - All Season Premium Bed Blanket (Full/Queen, Emerald)</t>
+  </si>
+  <si>
+    <t>YIHONG Set of 8 Stainless Steel Straws Ultra Long 10.5 Inch Drinking Metal Straws For Tumblers Rumblers Cold Beverage (4 Straight|4 Bent|2 Brushes)</t>
+  </si>
+  <si>
+    <t>DREAMFLYLIFE Luxury Fleece Blanket 380GSM Thick Blanket Super Soft Blanket Bed Warm Blanket Couch Blanket Winter Dark Grey Throw-Size, 50x61 in</t>
+  </si>
+  <si>
+    <t>Cat People</t>
+  </si>
+  <si>
+    <t>Hummingbird Glass Straws Clear Bent 9" x 9.5 mm…</t>
+  </si>
+  <si>
+    <t>Homfy Premium Cotton Pillows for Sleeping, Bed Pillows Queen Set of 2 with Medium Softness, Hypoallergenic and Breathable</t>
+  </si>
+  <si>
+    <t>Beyond the Mat</t>
+  </si>
+  <si>
+    <t>Shilucheng Luxury Fleece Blanket Super Soft and Warm Fuzzy Plush Lightweight Queen Couch Bed Blankets - Pink</t>
+  </si>
+  <si>
+    <t>Utopia Kitchen 6 Pieces Bowl Set - Dishwasher Safe Opal Glassware - Microwave/Oven Friendly</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1296,9 @@
       <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -1283,7 +1309,9 @@
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
@@ -1294,7 +1322,9 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
@@ -1305,7 +1335,9 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
@@ -1316,7 +1348,9 @@
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
@@ -1327,7 +1361,9 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
@@ -1336,9 +1372,11 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
@@ -1349,7 +1387,9 @@
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
@@ -1358,9 +1398,11 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
@@ -1371,7 +1413,9 @@
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>

</xml_diff>